<commit_message>
Add the develop branch
</commit_message>
<xml_diff>
--- a/tests/utils/study_inputs/study_bielvel_sobieski.xlsx
+++ b/tests/utils/study_inputs/study_bielvel_sobieski.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francois.gallard\Documents\workspace\GEMS\gems\utils\tests\study_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francois.gallard\Documents\workspace\GEMS\tests\utils\study_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="7140" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SobieskiStructure" sheetId="1" r:id="rId1"/>
-    <sheet name="SobieskiAerodynamics" sheetId="2" r:id="rId2"/>
+    <sheet name="SobieskiAerodynamics" sheetId="2" r:id="rId1"/>
+    <sheet name="SobieskiStructure" sheetId="1" r:id="rId2"/>
     <sheet name="SobieskiPropulsion" sheetId="4" r:id="rId3"/>
     <sheet name="SobieskiMission" sheetId="5" r:id="rId4"/>
     <sheet name="ScenarioStructure" sheetId="6" r:id="rId5"/>
@@ -495,70 +495,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -652,6 +588,70 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update from internal repository
</commit_message>
<xml_diff>
--- a/tests/utils/study_inputs/study_bielvel_sobieski.xlsx
+++ b/tests/utils/study_inputs/study_bielvel_sobieski.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="7140" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SobieskiAerodynamics" sheetId="2" r:id="rId1"/>
@@ -31,33 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
   <si>
     <t>Outputs</t>
   </si>
   <si>
     <t>Inputs</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>z</t>
   </si>
   <si>
     <t>Objective function</t>
@@ -495,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,84 +489,47 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>27</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -599,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -611,47 +553,47 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -661,10 +603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,81 +618,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -762,41 +667,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -816,41 +721,41 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -863,48 +768,48 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -924,41 +829,41 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -981,75 +886,75 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
         <v>40</v>
       </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>